<commit_message>
Update closes zones list
</commit_message>
<xml_diff>
--- a/src/misc/closed/ktes.xlsx
+++ b/src/misc/closed/ktes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My\Repo\kte\src\misc\closed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7812F438-2830-4061-A641-86ECCEFAD10B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D9C025-83A8-4E60-B81F-BAAD1AA1EE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="25320" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2022-12-06" sheetId="2" r:id="rId1"/>
-    <sheet name="2022-11-18" sheetId="1" r:id="rId2"/>
+    <sheet name="2022-12-21" sheetId="3" r:id="rId1"/>
+    <sheet name="2022-12-06" sheetId="2" r:id="rId2"/>
+    <sheet name="2022-11-18" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
   <si>
     <t>FILE</t>
   </si>
@@ -640,7 +641,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -668,6 +669,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1022,11 +1026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48541C13-6117-4C68-80CC-02D601E23A65}">
-  <dimension ref="A1:O31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFB80B4-2E37-41E5-96C5-D4D77DCB5591}">
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,6 +1099,843 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9">
+        <v>9</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9">
+        <v>6</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9">
+        <v>3</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9">
+        <v>9</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9">
+        <v>4</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9">
+        <v>5</v>
+      </c>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9">
+        <v>6</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9">
+        <v>5</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>16</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9">
+        <v>6</v>
+      </c>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9">
+        <v>8</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9">
+        <v>6</v>
+      </c>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9">
+        <v>6</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>19</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>20</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9">
+        <v>7</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9">
+        <v>4</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9">
+        <v>5</v>
+      </c>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9">
+        <v>5</v>
+      </c>
+      <c r="D26" s="9">
+        <v>7</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9">
+        <v>4</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9">
+        <v>6</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9">
+        <v>4</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9">
+        <v>7</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9">
+        <v>5</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9">
+        <v>4</v>
+      </c>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>25</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>26</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>28</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9">
+        <v>8</v>
+      </c>
+      <c r="L31" s="9">
+        <v>3</v>
+      </c>
+      <c r="M31" s="9">
+        <v>9</v>
+      </c>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>29</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9">
+        <v>6</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>30</v>
+      </c>
+      <c r="B33" s="9">
+        <v>8</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9">
+        <v>7</v>
+      </c>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="10">
+        <f>COUNTA(B2:B33)</f>
+        <v>9</v>
+      </c>
+      <c r="C34" s="10">
+        <f t="shared" ref="C34:O34" si="0">COUNTA(C2:C33)</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G34" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I34" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K34" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L34" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M34" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N34" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O34" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48541C13-6117-4C68-80CC-02D601E23A65}">
+  <dimension ref="A1:O31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:O31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>0</v>
       </c>
@@ -1793,7 +2634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
Report on closed zones
</commit_message>
<xml_diff>
--- a/src/misc/closed/ktes.xlsx
+++ b/src/misc/closed/ktes.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My\Repo\kte\src\misc\closed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D9C025-83A8-4E60-B81F-BAAD1AA1EE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="25320" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="25320" windowHeight="15210"/>
   </bookViews>
   <sheets>
-    <sheet name="2022-12-21" sheetId="3" r:id="rId1"/>
-    <sheet name="2022-12-06" sheetId="2" r:id="rId2"/>
-    <sheet name="2022-11-18" sheetId="1" r:id="rId3"/>
+    <sheet name="2023-02-02" sheetId="4" r:id="rId1"/>
+    <sheet name="2022-12-21" sheetId="3" r:id="rId2"/>
+    <sheet name="2022-12-06" sheetId="2" r:id="rId3"/>
+    <sheet name="2022-11-18" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="30">
   <si>
     <t>FILE</t>
   </si>
@@ -117,11 +117,17 @@
   <si>
     <t>st3@b</t>
   </si>
+  <si>
+    <t>st1@b</t>
+  </si>
+  <si>
+    <t>9+10+11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1026,10 +1032,919 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFB80B4-2E37-41E5-96C5-D4D77DCB5591}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9">
+        <v>9</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9">
+        <v>6</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
+        <v>3</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9">
+        <v>9</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9">
+        <v>4</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9">
+        <v>5</v>
+      </c>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9">
+        <v>7</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
+        <v>6</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9">
+        <v>5</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>16</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9">
+        <v>6</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9">
+        <v>8</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9">
+        <v>6</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>17</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
+        <v>6</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>18</v>
+      </c>
+      <c r="B24" s="9">
+        <v>6</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>19</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9">
+        <v>5</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>20</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>21</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9">
+        <v>7</v>
+      </c>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>22</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>23</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9">
+        <v>3</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9">
+        <v>4</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>24</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9">
+        <v>7</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9">
+        <v>4</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9">
+        <v>5</v>
+      </c>
+      <c r="O30" s="9"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9">
+        <v>5</v>
+      </c>
+      <c r="D31" s="9">
+        <v>7</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9">
+        <v>4</v>
+      </c>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9">
+        <v>6</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9">
+        <v>4</v>
+      </c>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9">
+        <v>7</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9">
+        <v>5</v>
+      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9">
+        <v>4</v>
+      </c>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>25</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>26</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>27</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9">
+        <v>2</v>
+      </c>
+      <c r="J36" s="9">
+        <v>6</v>
+      </c>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>28</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>29</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9">
+        <v>6</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>30</v>
+      </c>
+      <c r="B39" s="9">
+        <v>8</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9">
+        <v>7</v>
+      </c>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -1862,8 +2777,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48541C13-6117-4C68-80CC-02D601E23A65}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2634,8 +3549,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
Update Closed zone table
</commit_message>
<xml_diff>
--- a/src/misc/closed/ktes.xlsx
+++ b/src/misc/closed/ktes.xlsx
@@ -12,13 +12,14 @@
     <workbookView xWindow="-60" yWindow="-60" windowWidth="25320" windowHeight="15210"/>
   </bookViews>
   <sheets>
-    <sheet name="2023-02-03" sheetId="5" r:id="rId1"/>
-    <sheet name="2023-02-02" sheetId="4" r:id="rId2"/>
-    <sheet name="2022-12-21" sheetId="3" r:id="rId3"/>
-    <sheet name="2022-12-06" sheetId="2" r:id="rId4"/>
-    <sheet name="2022-11-18" sheetId="1" r:id="rId5"/>
+    <sheet name="2023-02-17" sheetId="6" r:id="rId1"/>
+    <sheet name="2023-02-03" sheetId="5" r:id="rId2"/>
+    <sheet name="2023-02-02" sheetId="4" r:id="rId3"/>
+    <sheet name="2022-12-21" sheetId="3" r:id="rId4"/>
+    <sheet name="2022-12-06" sheetId="2" r:id="rId5"/>
+    <sheet name="2022-11-18" sheetId="1" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="32">
   <si>
     <t>FILE</t>
   </si>
@@ -123,6 +124,12 @@
   </si>
   <si>
     <t>9+10+11</t>
+  </si>
+  <si>
+    <t>6+10</t>
+  </si>
+  <si>
+    <t>7+11</t>
   </si>
 </sst>
 </file>
@@ -1034,9 +1041,773 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9">
+        <v>9</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9">
+        <v>6</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
+        <v>3</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9">
+        <v>4</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9">
+        <v>5</v>
+      </c>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9">
+        <v>7</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9">
+        <v>10</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
+        <v>6</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9">
+        <v>5</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9">
+        <v>6</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>17</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9">
+        <v>7</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9">
+        <v>6</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
+      <c r="B20" s="9">
+        <v>6</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>19</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
+        <v>5</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>20</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
+        <v>7</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9">
+        <v>9</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9">
+        <v>3</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9">
+        <v>4</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>24</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9">
+        <v>7</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9">
+        <v>4</v>
+      </c>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9">
+        <v>5</v>
+      </c>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>25</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>26</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>27</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9">
+        <v>3</v>
+      </c>
+      <c r="J29" s="9">
+        <v>8</v>
+      </c>
+      <c r="K29" s="9">
+        <v>2</v>
+      </c>
+      <c r="L29" s="9">
+        <v>7</v>
+      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>28</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9">
+        <v>7</v>
+      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>29</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9">
+        <v>6</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>30</v>
+      </c>
+      <c r="B32" s="9">
+        <v>8</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9">
+        <v>7</v>
+      </c>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1953,7 +2724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
@@ -2862,7 +3633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
@@ -3699,7 +4470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
@@ -4471,7 +5242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>